<commit_message>
collection(list,set,map) & Utility homework
</commit_message>
<xml_diff>
--- a/Kosta/20172.xlsx
+++ b/Kosta/20172.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>가입 시 수집</t>
-  </si>
-  <si>
-    <t>비밀번호</t>
   </si>
   <si>
     <t>USER_PW</t>
@@ -682,6 +679,10 @@
   </si>
   <si>
     <t>not null</t>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1113,12 +1114,78 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1134,83 +1201,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,17 +1532,17 @@
   <dimension ref="B1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.625" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.625" style="4" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
@@ -1555,185 +1556,185 @@
   <sheetData>
     <row r="1" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="69" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
+      <c r="B2" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="75" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>111</v>
       </c>
       <c r="G2" s="71"/>
-      <c r="H2" s="76">
+      <c r="H2" s="79">
         <v>27</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="46"/>
       <c r="L2" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
+      <c r="B3" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="71"/>
-      <c r="H3" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
+      <c r="H3" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="46"/>
       <c r="L3" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M3" s="28">
         <v>42971</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="71" t="s">
-        <v>115</v>
-      </c>
       <c r="G4" s="71"/>
-      <c r="H4" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
+      <c r="H4" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="47"/>
       <c r="L4" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M4" s="28">
         <v>42971</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
+      <c r="B5" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="73"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
       <c r="K5" s="77"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="22"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66" t="s">
+      <c r="C7" s="58"/>
+      <c r="D7" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="48" t="s">
+      <c r="H7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="M7" s="48" t="s">
+      <c r="K7" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="M7" s="53" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="39">
         <v>1</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="41" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="43" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I9" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J9" s="42" t="s">
         <v>5</v>
@@ -1749,25 +1750,25 @@
         <v>2</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="H10" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>5</v>
@@ -1783,25 +1784,25 @@
         <v>3</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="H11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>5</v>
@@ -1817,28 +1818,28 @@
         <v>4</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="H12" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>4</v>
@@ -1851,28 +1852,28 @@
         <v>5</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="H13" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>4</v>
@@ -1885,31 +1886,31 @@
         <v>6</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -1919,25 +1920,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>5</v>
@@ -1953,26 +1954,26 @@
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="H16" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>4</v>
@@ -1985,29 +1986,29 @@
         <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="H17" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -2017,29 +2018,29 @@
         <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -2049,29 +2050,29 @@
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -2081,29 +2082,29 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -2113,29 +2114,29 @@
         <v>13</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I21" s="36"/>
       <c r="J21" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -2145,29 +2146,29 @@
         <v>14</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -2177,29 +2178,29 @@
         <v>15</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I23" s="36"/>
       <c r="J23" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -2209,29 +2210,29 @@
         <v>16</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I24" s="36"/>
       <c r="J24" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
@@ -2241,29 +2242,29 @@
         <v>17</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I25" s="36"/>
       <c r="J25" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -2273,29 +2274,29 @@
         <v>18</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I26" s="36"/>
       <c r="J26" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -2305,69 +2306,69 @@
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I27" s="36"/>
       <c r="J27" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
@@ -2375,7 +2376,7 @@
       <c r="C29" s="11"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -2387,245 +2388,245 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="56">
+      <c r="B30" s="59">
         <v>13</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="J30" s="59" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L30" s="29"/>
       <c r="M30" s="29"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="58"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
+        <v>26</v>
+      </c>
+      <c r="H31" s="52"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
       <c r="K31" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L31" s="30"/>
       <c r="M31" s="30"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="56">
+      <c r="B32" s="59">
         <v>14</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="J32" s="59" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="H32" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L32" s="29"/>
       <c r="M32" s="29"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="58"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="63"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
+        <v>31</v>
+      </c>
+      <c r="H33" s="52"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
       <c r="K33" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="56">
+      <c r="B34" s="59">
         <v>15</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" s="62" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="H34" s="51" t="s">
+        <v>36</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="J34" s="59" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="J34" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L34" s="29"/>
       <c r="M34" s="29"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="58"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="63"/>
+        <v>35</v>
+      </c>
+      <c r="H35" s="52"/>
       <c r="I35" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J35" s="61"/>
+        <v>127</v>
+      </c>
+      <c r="J35" s="50"/>
       <c r="K35" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="56">
+      <c r="B36" s="59">
         <v>16</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="62" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="H36" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="J36" s="59" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L36" s="29"/>
       <c r="M36" s="29"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="58"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H37" s="63"/>
+        <v>40</v>
+      </c>
+      <c r="H37" s="52"/>
       <c r="I37" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J37" s="61"/>
+        <v>127</v>
+      </c>
+      <c r="J37" s="50"/>
       <c r="K37" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
@@ -2635,288 +2636,308 @@
         <v>17</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="H38" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J38" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B39" s="56">
+      <c r="B39" s="59">
         <v>18</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H39" s="62" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="H39" s="51" t="s">
+        <v>50</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="J39" s="59" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="J39" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L39" s="29"/>
       <c r="M39" s="29"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B40" s="57"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H40" s="64"/>
+        <v>48</v>
+      </c>
+      <c r="H40" s="55"/>
       <c r="I40" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="J40" s="60"/>
+        <v>127</v>
+      </c>
+      <c r="J40" s="49"/>
       <c r="K40" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L40" s="31"/>
       <c r="M40" s="31"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" s="58"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H41" s="63"/>
+        <v>49</v>
+      </c>
+      <c r="H41" s="52"/>
       <c r="I41" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J41" s="61"/>
+        <v>127</v>
+      </c>
+      <c r="J41" s="50"/>
       <c r="K41" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B42" s="56">
+      <c r="B42" s="59">
         <v>19</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H42" s="78" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="H42" s="63" t="s">
+        <v>58</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="J42" s="59" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+      <c r="J42" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L42" s="29"/>
       <c r="M42" s="29"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B43" s="57"/>
+      <c r="B43" s="61"/>
       <c r="C43" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H43" s="79"/>
+        <v>55</v>
+      </c>
+      <c r="H43" s="64"/>
       <c r="I43" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="J43" s="60"/>
+        <v>127</v>
+      </c>
+      <c r="J43" s="49"/>
       <c r="K43" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B44" s="57"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="H44" s="79"/>
+        <v>56</v>
+      </c>
+      <c r="H44" s="64"/>
       <c r="I44" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="J44" s="60"/>
+        <v>127</v>
+      </c>
+      <c r="J44" s="49"/>
       <c r="K44" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B45" s="58"/>
+      <c r="B45" s="60"/>
       <c r="C45" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H45" s="80"/>
+        <v>57</v>
+      </c>
+      <c r="H45" s="65"/>
       <c r="I45" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J45" s="61"/>
+        <v>127</v>
+      </c>
+      <c r="J45" s="50"/>
       <c r="K45" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L45" s="30"/>
       <c r="M45" s="30"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="J42:J45"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B39:B41"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
@@ -2930,31 +2951,11 @@
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="J32:J33"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:M5"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="J42:J45"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="J36:J37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>